<commit_message>
Added perliminary results on the execution time for analysis
</commit_message>
<xml_diff>
--- a/Dados Perliminares de Tempo.xlsx
+++ b/Dados Perliminares de Tempo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renato\CLionProjects\cp2020-2021_g26_45616_52360_52393\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15CC3260-1F7D-4E74-B2FD-31DF4D7D9561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD1E0CB-D102-4E9A-9892-DE7747E32AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{4BADC3A3-214E-4F71-BF37-35E3E3FF7E6D}"/>
   </bookViews>
@@ -713,7 +713,7 @@
   <dimension ref="B3:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update de dados perliminares com 2 ficheiros (teste2 e teste7)
</commit_message>
<xml_diff>
--- a/Dados Perliminares de Tempo.xlsx
+++ b/Dados Perliminares de Tempo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renato\CLionProjects\cp2020-2021_g26_45616_52360_52393\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD1E0CB-D102-4E9A-9892-DE7747E32AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC6DE90-BABD-4C65-84D3-2AFFFBBDB71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{4BADC3A3-214E-4F71-BF37-35E3E3FF7E6D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="92">
   <si>
     <t>Seq</t>
   </si>
@@ -178,14 +178,154 @@
   </si>
   <si>
     <t>8.409981</t>
+  </si>
+  <si>
+    <t>8.443763</t>
+  </si>
+  <si>
+    <t>8.436171</t>
+  </si>
+  <si>
+    <t>8.452003</t>
+  </si>
+  <si>
+    <t>8.456196</t>
+  </si>
+  <si>
+    <t>8.316259</t>
+  </si>
+  <si>
+    <t>8.324851</t>
+  </si>
+  <si>
+    <t>2 ficheiros</t>
+  </si>
+  <si>
+    <t>1.263608</t>
+  </si>
+  <si>
+    <t>1.297149</t>
+  </si>
+  <si>
+    <t>1.313690</t>
+  </si>
+  <si>
+    <t>1.309831</t>
+  </si>
+  <si>
+    <t>1.293098</t>
+  </si>
+  <si>
+    <t>1.296992</t>
+  </si>
+  <si>
+    <t>1.291525</t>
+  </si>
+  <si>
+    <t>1.288420</t>
+  </si>
+  <si>
+    <t>1.280386</t>
+  </si>
+  <si>
+    <t>1.276798</t>
+  </si>
+  <si>
+    <t>1 ficheiro</t>
+  </si>
+  <si>
+    <t>69.461413</t>
+  </si>
+  <si>
+    <t>69.489945</t>
+  </si>
+  <si>
+    <t>69.416433</t>
+  </si>
+  <si>
+    <t>seq</t>
+  </si>
+  <si>
+    <t>par</t>
+  </si>
+  <si>
+    <t>69.409300</t>
+  </si>
+  <si>
+    <t>teste8</t>
+  </si>
+  <si>
+    <t>teste9</t>
+  </si>
+  <si>
+    <t>69.440620</t>
+  </si>
+  <si>
+    <t>69.564721</t>
+  </si>
+  <si>
+    <t>69.680427</t>
+  </si>
+  <si>
+    <t>69.517126</t>
+  </si>
+  <si>
+    <t>69.617721</t>
+  </si>
+  <si>
+    <t>69.422080</t>
+  </si>
+  <si>
+    <t>10.377236</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 7 4800HS</t>
+  </si>
+  <si>
+    <t>16 processadores logicos</t>
+  </si>
+  <si>
+    <t>10.122220</t>
+  </si>
+  <si>
+    <t>11.753683</t>
+  </si>
+  <si>
+    <t>10.747296</t>
+  </si>
+  <si>
+    <t>10.274935</t>
+  </si>
+  <si>
+    <t>10.070961</t>
+  </si>
+  <si>
+    <t>10.542535</t>
+  </si>
+  <si>
+    <t>10.746904</t>
+  </si>
+  <si>
+    <t>10.769529</t>
+  </si>
+  <si>
+    <t>10.691818</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -201,7 +341,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -320,23 +460,104 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -348,25 +569,38 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -379,23 +613,62 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,44 +983,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE47BE7D-00DC-4DA1-9970-9DCED18DDF0E}">
-  <dimension ref="B3:F22"/>
+  <dimension ref="B1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.21875" customWidth="1"/>
     <col min="6" max="6" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="1" t="s">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="11" t="s">
+      <c r="F3" s="23"/>
+      <c r="G3" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="20"/>
+      <c r="I3" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="20"/>
+    </row>
+    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>
@@ -760,164 +1059,204 @@
       <c r="E5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="1"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="1"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>6</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="1"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>7</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="1"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>8</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>9</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G13" s="1"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>10</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="3"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C15" t="e">
         <f>AVERAGE(C5:C14)</f>
         <v>#DIV/0!</v>
@@ -927,31 +1266,202 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
+    <row r="17" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+      <c r="D19" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
+      <c r="D20" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
+      <c r="D21" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>47</v>
       </c>
+      <c r="D22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added perliminar times from test_09
</commit_message>
<xml_diff>
--- a/Dados Perliminares de Tempo.xlsx
+++ b/Dados Perliminares de Tempo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renato\CLionProjects\cp2020-2021_g26_45616_52360_52393\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB677550-53F0-4BB1-B5D6-A212D04D978B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80D9339-2A7E-4E35-ACC7-211D77701341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{4BADC3A3-214E-4F71-BF37-35E3E3FF7E6D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="20">
   <si>
     <t>AMD Ryzen 7 4800HS</t>
   </si>
@@ -89,13 +89,27 @@
   <si>
     <t>3 FILES</t>
   </si>
+  <si>
+    <t>16 positions</t>
+  </si>
+  <si>
+    <t>17 positions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -111,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -620,11 +634,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -644,35 +695,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -738,6 +765,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -745,6 +819,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1061,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE47BE7D-00DC-4DA1-9970-9DCED18DDF0E}">
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1084,115 +1161,123 @@
     <col min="13" max="13" width="12.77734375" customWidth="1"/>
     <col min="14" max="14" width="14.6640625" customWidth="1"/>
     <col min="15" max="15" width="11.88671875" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" customWidth="1"/>
-    <col min="17" max="17" width="14.77734375" customWidth="1"/>
-    <col min="18" max="18" width="15.5546875" customWidth="1"/>
+    <col min="16" max="17" width="14.33203125" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5546875" customWidth="1"/>
+    <col min="20" max="20" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="7" t="s">
+      <c r="Q1" s="39"/>
+    </row>
+    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q2" s="39"/>
+    </row>
+    <row r="3" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="45"/>
+      <c r="E3" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="45"/>
+      <c r="G3" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="10" t="s">
+      <c r="H3" s="47"/>
+      <c r="I3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="10" t="s">
+      <c r="J3" s="47"/>
+      <c r="K3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="7" t="s">
+      <c r="L3" s="47"/>
+      <c r="M3" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="8"/>
-      <c r="O3" s="7" t="s">
+      <c r="N3" s="45"/>
+      <c r="O3" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="10" t="s">
+      <c r="P3" s="45"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="11"/>
-    </row>
-    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="23" t="s">
+      <c r="T3" s="47"/>
+    </row>
+    <row r="4" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="33" t="s">
+      <c r="J4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="32" t="s">
+      <c r="K4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="33" t="s">
+      <c r="L4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="32" t="s">
+      <c r="M4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="31" t="s">
+      <c r="N4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="32" t="s">
+      <c r="O4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="31" t="s">
+      <c r="P4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="32" t="s">
+      <c r="Q4" s="37"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="R4" s="33" t="s">
+      <c r="T4" s="25" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="14">
         <v>1</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="9">
         <v>4.2290580000000002</v>
       </c>
       <c r="D5" s="2">
@@ -1207,34 +1292,42 @@
       <c r="G5" s="3">
         <v>4.2218260000000001</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="7">
         <v>3.086354</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="12"/>
+      <c r="J5" s="7"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="27">
+      <c r="L5" s="7"/>
+      <c r="M5" s="19">
         <v>35.224710000000002</v>
       </c>
-      <c r="N5" s="28">
+      <c r="N5" s="20">
         <v>6.458469</v>
       </c>
       <c r="O5" s="3">
         <v>4.2218260000000001</v>
       </c>
-      <c r="P5" s="12">
+      <c r="P5" s="7">
         <v>3.086354</v>
       </c>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="12"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="20">
+      <c r="Q5" s="38"/>
+      <c r="R5" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="S5" s="3">
+        <v>1.1E-5</v>
+      </c>
+      <c r="T5" s="7">
+        <v>2.1480000000000002E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="49"/>
+      <c r="B6" s="12">
         <v>2</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="10">
         <v>4.2042070000000002</v>
       </c>
       <c r="D6" s="4">
@@ -1249,34 +1342,40 @@
       <c r="G6" s="3">
         <v>4.1967489999999996</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="7">
         <v>2.9564750000000002</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="12"/>
+      <c r="J6" s="7"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="12"/>
+      <c r="L6" s="7"/>
       <c r="M6" s="3">
         <v>35.109192</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="7">
         <v>6.3253219999999999</v>
       </c>
       <c r="O6" s="3">
         <v>4.1967489999999996</v>
       </c>
-      <c r="P6" s="12">
+      <c r="P6" s="7">
         <v>2.9564750000000002</v>
       </c>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="12"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="20">
+      <c r="Q6" s="38"/>
+      <c r="R6" s="42"/>
+      <c r="S6" s="3">
+        <v>1.1E-5</v>
+      </c>
+      <c r="T6" s="7">
+        <v>6.587E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="49"/>
+      <c r="B7" s="12">
         <v>3</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="10">
         <v>4.2019149999999996</v>
       </c>
       <c r="D7" s="4">
@@ -1291,34 +1390,40 @@
       <c r="G7" s="3">
         <v>4.20716</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="7">
         <v>3.0146310000000001</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="12"/>
+      <c r="J7" s="7"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="12"/>
+      <c r="L7" s="7"/>
       <c r="M7" s="3">
         <v>35.100942000000003</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="7">
         <v>6.2677849999999999</v>
       </c>
       <c r="O7" s="3">
         <v>4.20716</v>
       </c>
-      <c r="P7" s="12">
+      <c r="P7" s="7">
         <v>3.0146310000000001</v>
       </c>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="12"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="20">
+      <c r="Q7" s="38"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="T7" s="7">
+        <v>7.4819999999999999E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="49"/>
+      <c r="B8" s="12">
         <v>4</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="10">
         <v>4.234953</v>
       </c>
       <c r="D8" s="4">
@@ -1333,34 +1438,40 @@
       <c r="G8" s="3">
         <v>4.220224</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="7">
         <v>2.9678469999999999</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="12"/>
+      <c r="J8" s="7"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="12"/>
+      <c r="L8" s="7"/>
       <c r="M8" s="3">
         <v>35.095021000000003</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8" s="7">
         <v>6.2611319999999999</v>
       </c>
       <c r="O8" s="3">
         <v>4.220224</v>
       </c>
-      <c r="P8" s="12">
+      <c r="P8" s="7">
         <v>2.9678469999999999</v>
       </c>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="12"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="20">
+      <c r="Q8" s="38"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="3">
+        <v>1.1E-5</v>
+      </c>
+      <c r="T8" s="7">
+        <v>1.81E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="49"/>
+      <c r="B9" s="12">
         <v>5</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="10">
         <v>4.211398</v>
       </c>
       <c r="D9" s="4">
@@ -1375,34 +1486,40 @@
       <c r="G9" s="3">
         <v>4.1599180000000002</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="7">
         <v>3.0438670000000001</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="12"/>
+      <c r="J9" s="7"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="12"/>
+      <c r="L9" s="7"/>
       <c r="M9" s="3">
         <v>35.194079000000002</v>
       </c>
-      <c r="N9" s="12">
+      <c r="N9" s="7">
         <v>6.316573</v>
       </c>
       <c r="O9" s="3">
         <v>4.1599180000000002</v>
       </c>
-      <c r="P9" s="12">
+      <c r="P9" s="7">
         <v>3.0438670000000001</v>
       </c>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="12"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="20">
+      <c r="Q9" s="38"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="3">
+        <v>1.1E-5</v>
+      </c>
+      <c r="T9" s="7">
+        <v>6.3400000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="49"/>
+      <c r="B10" s="12">
         <v>6</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="10">
         <v>4.2320339999999996</v>
       </c>
       <c r="D10" s="4">
@@ -1417,34 +1534,40 @@
       <c r="G10" s="3">
         <v>4.1979439999999997</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="7">
         <v>3.0445630000000001</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="12"/>
+      <c r="J10" s="7"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="12"/>
+      <c r="L10" s="7"/>
       <c r="M10" s="3">
         <v>35.181164000000003</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="7">
         <v>6.9119440000000001</v>
       </c>
       <c r="O10" s="3">
         <v>4.1979439999999997</v>
       </c>
-      <c r="P10" s="12">
+      <c r="P10" s="7">
         <v>3.0445630000000001</v>
       </c>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="12"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="20">
+      <c r="Q10" s="38"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="3">
+        <v>1.1E-5</v>
+      </c>
+      <c r="T10" s="7">
+        <v>1.621E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="49"/>
+      <c r="B11" s="12">
         <v>7</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="10">
         <v>4.2398119999999997</v>
       </c>
       <c r="D11" s="4">
@@ -1459,34 +1582,40 @@
       <c r="G11" s="3">
         <v>4.1616780000000002</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="7">
         <v>2.9294349999999998</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="12"/>
+      <c r="J11" s="7"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="12"/>
+      <c r="L11" s="7"/>
       <c r="M11" s="3">
         <v>35.241520000000001</v>
       </c>
-      <c r="N11" s="12">
+      <c r="N11" s="7">
         <v>6.4361220000000001</v>
       </c>
       <c r="O11" s="3">
         <v>4.1616780000000002</v>
       </c>
-      <c r="P11" s="12">
+      <c r="P11" s="7">
         <v>2.9294349999999998</v>
       </c>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="12"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="20">
+      <c r="Q11" s="38"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="T11" s="7">
+        <v>7.4710000000000002E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="49"/>
+      <c r="B12" s="12">
         <v>8</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="10">
         <v>4.213006</v>
       </c>
       <c r="D12" s="4">
@@ -1501,34 +1630,40 @@
       <c r="G12" s="3">
         <v>4.2769399999999997</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="7">
         <v>2.8758550000000001</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="12"/>
+      <c r="J12" s="7"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="12"/>
+      <c r="L12" s="7"/>
       <c r="M12" s="3">
         <v>35.265450000000001</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="7">
         <v>6.0774379999999999</v>
       </c>
       <c r="O12" s="3">
         <v>4.2769399999999997</v>
       </c>
-      <c r="P12" s="12">
+      <c r="P12" s="7">
         <v>2.8758550000000001</v>
       </c>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="12"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="20">
+      <c r="Q12" s="38"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="3">
+        <v>1.1E-5</v>
+      </c>
+      <c r="T12" s="7">
+        <v>7.4710000000000002E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="49"/>
+      <c r="B13" s="12">
         <v>9</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="10">
         <v>4.2277509999999996</v>
       </c>
       <c r="D13" s="4">
@@ -1543,287 +1678,319 @@
       <c r="G13" s="3">
         <v>4.2313939999999999</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="7">
         <v>2.853167</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="12"/>
+      <c r="J13" s="7"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="12"/>
+      <c r="L13" s="7"/>
       <c r="M13" s="3">
         <v>35.220028999999997</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N13" s="7">
         <v>6.6786669999999999</v>
       </c>
       <c r="O13" s="3">
         <v>4.2313939999999999</v>
       </c>
-      <c r="P13" s="12">
+      <c r="P13" s="7">
         <v>2.853167</v>
       </c>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="12"/>
-    </row>
-    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16"/>
-      <c r="B14" s="21">
+      <c r="Q13" s="38"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="3">
+        <v>1.1E-5</v>
+      </c>
+      <c r="T13" s="7">
+        <v>1.4610000000000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="50"/>
+      <c r="B14" s="13">
         <v>10</v>
       </c>
-      <c r="C14" s="37">
+      <c r="C14" s="29">
         <v>4.22736</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="30">
         <v>0.82677900000000004</v>
       </c>
-      <c r="E14" s="39">
+      <c r="E14" s="31">
         <v>35.111255</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="30">
         <v>6.6003360000000004</v>
       </c>
-      <c r="G14" s="39">
+      <c r="G14" s="31">
         <v>4.223471</v>
       </c>
-      <c r="H14" s="40">
+      <c r="H14" s="32">
         <v>2.8457180000000002</v>
       </c>
-      <c r="I14" s="39"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="39">
+      <c r="I14" s="31"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="31">
         <v>35.111255</v>
       </c>
-      <c r="N14" s="40">
+      <c r="N14" s="32">
         <v>6.6003360000000004</v>
       </c>
-      <c r="O14" s="39">
+      <c r="O14" s="31">
         <v>4.223471</v>
       </c>
-      <c r="P14" s="40">
+      <c r="P14" s="32">
         <v>2.8457180000000002</v>
       </c>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="40"/>
-    </row>
-    <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="Q14" s="38"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="31">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="T14" s="32">
+        <v>1.488E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="41">
+      <c r="B15" s="44"/>
+      <c r="C15" s="33">
         <f>AVERAGE(C5:C14)</f>
         <v>4.2221493999999993</v>
       </c>
-      <c r="D15" s="42">
-        <f t="shared" ref="D15:R15" si="0">AVERAGE(D5:D14)</f>
+      <c r="D15" s="34">
+        <f t="shared" ref="D15:T15" si="0">AVERAGE(D5:D14)</f>
         <v>0.89827919999999994</v>
       </c>
-      <c r="E15" s="41">
+      <c r="E15" s="33">
         <f t="shared" si="0"/>
         <v>35.174336200000006</v>
       </c>
-      <c r="F15" s="42">
+      <c r="F15" s="34">
         <f t="shared" si="0"/>
         <v>6.4333787999999998</v>
       </c>
-      <c r="G15" s="41">
+      <c r="G15" s="33">
         <f t="shared" si="0"/>
         <v>4.2097303999999998</v>
       </c>
-      <c r="H15" s="42">
+      <c r="H15" s="34">
         <f t="shared" si="0"/>
         <v>2.9617912</v>
       </c>
-      <c r="I15" s="41" t="e">
+      <c r="I15" s="33" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J15" s="42" t="e">
+      <c r="J15" s="34" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K15" s="41" t="e">
+      <c r="K15" s="33" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L15" s="42" t="e">
+      <c r="L15" s="34" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M15" s="41">
+      <c r="M15" s="33">
         <f t="shared" si="0"/>
         <v>35.174336200000006</v>
       </c>
-      <c r="N15" s="42">
+      <c r="N15" s="34">
         <f t="shared" si="0"/>
         <v>6.4333787999999998</v>
       </c>
-      <c r="O15" s="41">
-        <f t="shared" si="0"/>
+      <c r="O15" s="33">
+        <f>AVERAGE(O5:O14)</f>
         <v>4.2097303999999998</v>
       </c>
-      <c r="P15" s="42">
+      <c r="P15" s="34">
         <f t="shared" si="0"/>
         <v>2.9617912</v>
       </c>
-      <c r="Q15" s="41" t="e">
+      <c r="Q15" s="38"/>
+      <c r="R15" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="S15" s="33">
+        <f t="shared" ref="S15" si="1">AVERAGE(S5:S14)</f>
+        <v>1.0699999999999999E-5</v>
+      </c>
+      <c r="T15" s="34">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R15" s="42" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
+        <v>4.3879000000000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="43" t="str">
+      <c r="B16" s="45"/>
+      <c r="C16" s="52" t="str">
         <f>IMDIV(C15,D15)</f>
         <v>4,70026401590953</v>
       </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="43" t="str">
+      <c r="D16" s="53"/>
+      <c r="E16" s="52" t="str">
         <f>IMDIV(E15,F15)</f>
         <v>5,46747475836492</v>
       </c>
-      <c r="F16" s="44"/>
-      <c r="G16" s="43" t="str">
-        <f t="shared" ref="G16" si="1">IMDIV(G15,H15)</f>
+      <c r="F16" s="53"/>
+      <c r="G16" s="52" t="str">
+        <f>IMDIV(G15,H15)</f>
         <v>1,42134610974602</v>
       </c>
-      <c r="H16" s="44"/>
-      <c r="I16" s="43" t="e">
+      <c r="H16" s="53"/>
+      <c r="I16" s="52" t="e">
         <f t="shared" ref="I16" si="2">IMDIV(I15,J15)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J16" s="44"/>
-      <c r="K16" s="43" t="e">
+      <c r="J16" s="53"/>
+      <c r="K16" s="52" t="e">
         <f t="shared" ref="K16" si="3">IMDIV(K15,L15)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L16" s="44"/>
-      <c r="M16" s="43" t="str">
+      <c r="L16" s="53"/>
+      <c r="M16" s="52" t="str">
         <f t="shared" ref="M16" si="4">IMDIV(M15,N15)</f>
         <v>5,46747475836492</v>
       </c>
-      <c r="N16" s="44"/>
-      <c r="O16" s="43" t="str">
+      <c r="N16" s="53"/>
+      <c r="O16" s="52" t="str">
         <f t="shared" ref="O16" si="5">IMDIV(O15,P15)</f>
         <v>1,42134610974602</v>
       </c>
-      <c r="P16" s="44"/>
-      <c r="Q16" s="43" t="e">
-        <f t="shared" ref="Q16" si="6">IMDIV(Q15,R15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R16" s="45"/>
-    </row>
-    <row r="17" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="34" t="s">
+      <c r="P16" s="54"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="S16" s="52" t="str">
+        <f>IMDIV(S15,T15)</f>
+        <v>0,00243852412315686</v>
+      </c>
+      <c r="T16" s="54"/>
+    </row>
+    <row r="17" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q17" s="39"/>
+    </row>
+    <row r="18" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F18" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H18" s="31" t="s">
+      <c r="H18" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I18" s="32" t="s">
+      <c r="I18" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="J18" s="33" t="s">
+      <c r="J18" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="K18" s="32" t="s">
+      <c r="K18" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="L18" s="33" t="s">
+      <c r="L18" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="M18" s="35" t="s">
+      <c r="M18" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="N18" s="36" t="s">
+      <c r="N18" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="O18" s="32" t="s">
+      <c r="O18" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="P18" s="31" t="s">
+      <c r="P18" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Q18" s="32" t="s">
+      <c r="Q18" s="37"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="R18" s="33" t="s">
+      <c r="T18" s="25" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A19" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B19" s="16">
         <v>1</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="19">
         <v>8.4040909999999993</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="21">
         <v>1.2636080000000001</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="19">
         <v>69.461412999999993</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="20">
         <v>10.377236</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="10">
         <v>6.6805789999999998</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="7">
         <v>4.3654729999999997</v>
       </c>
       <c r="I19" s="3"/>
-      <c r="J19" s="12"/>
+      <c r="J19" s="7"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="27">
+      <c r="L19" s="7"/>
+      <c r="M19" s="19">
         <v>69.461412999999993</v>
       </c>
-      <c r="N19" s="28">
+      <c r="N19" s="20">
         <v>10.377236</v>
       </c>
-      <c r="O19" s="18">
+      <c r="O19" s="3">
         <v>6.6805789999999998</v>
       </c>
-      <c r="P19" s="12">
+      <c r="P19" s="7">
         <v>4.3654729999999997</v>
       </c>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="12"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="25">
+      <c r="Q19" s="38"/>
+      <c r="R19" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="S19" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="T19" s="7">
+        <v>1.25E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" s="49"/>
+      <c r="B20" s="17">
         <v>2</v>
       </c>
       <c r="C20" s="3">
@@ -1835,37 +2002,44 @@
       <c r="E20" s="3">
         <v>69.489945000000006</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="7">
         <v>10.12222</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="10">
         <v>6.6813589999999996</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="7">
         <v>4.4872519999999998</v>
       </c>
       <c r="I20" s="3"/>
-      <c r="J20" s="12"/>
+      <c r="J20" s="7"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="12"/>
+      <c r="L20" s="7"/>
       <c r="M20" s="3">
         <v>69.489945000000006</v>
       </c>
-      <c r="N20" s="12">
+      <c r="N20" s="7">
         <v>10.12222</v>
       </c>
-      <c r="O20" s="18">
+      <c r="O20" s="3">
         <v>6.6813589999999996</v>
       </c>
-      <c r="P20" s="12">
+      <c r="P20" s="7">
         <v>4.4872519999999998</v>
       </c>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="12"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="25">
+      <c r="Q20" s="38"/>
+      <c r="R20" s="42"/>
+      <c r="S20" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="T20" s="7">
+        <v>2.2620000000000001E-3</v>
+      </c>
+      <c r="V20" s="40"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A21" s="49"/>
+      <c r="B21" s="17">
         <v>3</v>
       </c>
       <c r="C21" s="3">
@@ -1877,37 +2051,43 @@
       <c r="E21" s="3">
         <v>69.416432999999998</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="7">
         <v>11.753683000000001</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="10">
         <v>6.7529510000000004</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="7">
         <v>4.3293169999999996</v>
       </c>
       <c r="I21" s="3"/>
-      <c r="J21" s="12"/>
+      <c r="J21" s="7"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="12"/>
+      <c r="L21" s="7"/>
       <c r="M21" s="3">
         <v>69.416432999999998</v>
       </c>
-      <c r="N21" s="12">
+      <c r="N21" s="7">
         <v>11.753683000000001</v>
       </c>
-      <c r="O21" s="18">
+      <c r="O21" s="3">
         <v>6.7529510000000004</v>
       </c>
-      <c r="P21" s="12">
+      <c r="P21" s="7">
         <v>4.3293169999999996</v>
       </c>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="12"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="25">
+      <c r="Q21" s="38"/>
+      <c r="R21" s="42"/>
+      <c r="S21" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="T21" s="7">
+        <v>2.137E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A22" s="49"/>
+      <c r="B22" s="17">
         <v>4</v>
       </c>
       <c r="C22" s="3">
@@ -1919,37 +2099,43 @@
       <c r="E22" s="3">
         <v>69.409300000000002</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="7">
         <v>10.747296</v>
       </c>
-      <c r="G22" s="18">
+      <c r="G22" s="10">
         <v>6.7511830000000002</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="7">
         <v>4.4122719999999997</v>
       </c>
       <c r="I22" s="3"/>
-      <c r="J22" s="12"/>
+      <c r="J22" s="7"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="12"/>
+      <c r="L22" s="7"/>
       <c r="M22" s="3">
         <v>69.409300000000002</v>
       </c>
-      <c r="N22" s="12">
+      <c r="N22" s="7">
         <v>10.747296</v>
       </c>
-      <c r="O22" s="18">
+      <c r="O22" s="3">
         <v>6.7511830000000002</v>
       </c>
-      <c r="P22" s="12">
+      <c r="P22" s="7">
         <v>4.4122719999999997</v>
       </c>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="12"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
-      <c r="B23" s="25">
+      <c r="Q22" s="38"/>
+      <c r="R22" s="42"/>
+      <c r="S22" s="3">
+        <v>1.1E-5</v>
+      </c>
+      <c r="T22" s="7">
+        <v>2.2060000000000001E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A23" s="49"/>
+      <c r="B23" s="17">
         <v>5</v>
       </c>
       <c r="C23" s="3">
@@ -1961,37 +2147,43 @@
       <c r="E23" s="3">
         <v>69.440619999999996</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="7">
         <v>10.274934999999999</v>
       </c>
-      <c r="G23" s="18">
+      <c r="G23" s="10">
         <v>6.7855920000000003</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="7">
         <v>4.358771</v>
       </c>
       <c r="I23" s="3"/>
-      <c r="J23" s="12"/>
+      <c r="J23" s="7"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="12"/>
+      <c r="L23" s="7"/>
       <c r="M23" s="3">
         <v>69.440619999999996</v>
       </c>
-      <c r="N23" s="12">
+      <c r="N23" s="7">
         <v>10.274934999999999</v>
       </c>
-      <c r="O23" s="18">
+      <c r="O23" s="3">
         <v>6.7855920000000003</v>
       </c>
-      <c r="P23" s="12">
+      <c r="P23" s="7">
         <v>4.358771</v>
       </c>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="12"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
-      <c r="B24" s="25">
+      <c r="Q23" s="38"/>
+      <c r="R23" s="42"/>
+      <c r="S23" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="T23" s="7">
+        <v>1.433E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A24" s="49"/>
+      <c r="B24" s="17">
         <v>6</v>
       </c>
       <c r="C24" s="3">
@@ -2003,37 +2195,43 @@
       <c r="E24" s="3">
         <v>69.564721000000006</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="7">
         <v>10.070961</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="10">
         <v>6.3858620000000004</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="7">
         <v>4.2449329999999996</v>
       </c>
       <c r="I24" s="3"/>
-      <c r="J24" s="12"/>
+      <c r="J24" s="7"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="12"/>
+      <c r="L24" s="7"/>
       <c r="M24" s="3">
         <v>69.564721000000006</v>
       </c>
-      <c r="N24" s="12">
+      <c r="N24" s="7">
         <v>10.070961</v>
       </c>
-      <c r="O24" s="18">
+      <c r="O24" s="3">
         <v>6.3858620000000004</v>
       </c>
-      <c r="P24" s="12">
+      <c r="P24" s="7">
         <v>4.2449329999999996</v>
       </c>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="12"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="25">
+      <c r="Q24" s="38"/>
+      <c r="R24" s="42"/>
+      <c r="S24" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="T24" s="7">
+        <v>1.6789999999999999E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A25" s="49"/>
+      <c r="B25" s="17">
         <v>7</v>
       </c>
       <c r="C25" s="3">
@@ -2045,37 +2243,43 @@
       <c r="E25" s="3">
         <v>69.680426999999995</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25" s="7">
         <v>10.542535000000001</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G25" s="10">
         <v>6.3877220000000001</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="7">
         <v>4.3251090000000003</v>
       </c>
       <c r="I25" s="3"/>
-      <c r="J25" s="12"/>
+      <c r="J25" s="7"/>
       <c r="K25" s="3"/>
-      <c r="L25" s="12"/>
+      <c r="L25" s="7"/>
       <c r="M25" s="3">
         <v>69.680426999999995</v>
       </c>
-      <c r="N25" s="12">
+      <c r="N25" s="7">
         <v>10.542535000000001</v>
       </c>
-      <c r="O25" s="18">
+      <c r="O25" s="3">
         <v>6.3877220000000001</v>
       </c>
-      <c r="P25" s="12">
+      <c r="P25" s="7">
         <v>4.3251090000000003</v>
       </c>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="12"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
-      <c r="B26" s="25">
+      <c r="Q25" s="38"/>
+      <c r="R25" s="42"/>
+      <c r="S25" s="3">
+        <v>1.1E-5</v>
+      </c>
+      <c r="T25" s="7">
+        <v>7.6990000000000001E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A26" s="49"/>
+      <c r="B26" s="17">
         <v>8</v>
       </c>
       <c r="C26" s="3">
@@ -2087,37 +2291,43 @@
       <c r="E26" s="3">
         <v>69.517126000000005</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="7">
         <v>10.746904000000001</v>
       </c>
-      <c r="G26" s="18">
+      <c r="G26" s="10">
         <v>6.4815839999999998</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="7">
         <v>4.1902410000000003</v>
       </c>
       <c r="I26" s="3"/>
-      <c r="J26" s="12"/>
+      <c r="J26" s="7"/>
       <c r="K26" s="3"/>
-      <c r="L26" s="12"/>
+      <c r="L26" s="7"/>
       <c r="M26" s="3">
         <v>69.517126000000005</v>
       </c>
-      <c r="N26" s="12">
+      <c r="N26" s="7">
         <v>10.746904000000001</v>
       </c>
-      <c r="O26" s="18">
+      <c r="O26" s="3">
         <v>6.4815839999999998</v>
       </c>
-      <c r="P26" s="12">
+      <c r="P26" s="7">
         <v>4.1902410000000003</v>
       </c>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="12"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
-      <c r="B27" s="25">
+      <c r="Q26" s="38"/>
+      <c r="R26" s="42"/>
+      <c r="S26" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="T26" s="7">
+        <v>1.3550000000000001E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A27" s="49"/>
+      <c r="B27" s="17">
         <v>9</v>
       </c>
       <c r="C27" s="3">
@@ -2129,37 +2339,43 @@
       <c r="E27" s="3">
         <v>69.617721000000003</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="7">
         <v>10.769529</v>
       </c>
-      <c r="G27" s="18">
+      <c r="G27" s="10">
         <v>6.7411089999999998</v>
       </c>
-      <c r="H27" s="12">
+      <c r="H27" s="7">
         <v>4.1781940000000004</v>
       </c>
       <c r="I27" s="3"/>
-      <c r="J27" s="12"/>
+      <c r="J27" s="7"/>
       <c r="K27" s="3"/>
-      <c r="L27" s="12"/>
+      <c r="L27" s="7"/>
       <c r="M27" s="3">
         <v>69.617721000000003</v>
       </c>
-      <c r="N27" s="12">
+      <c r="N27" s="7">
         <v>10.769529</v>
       </c>
-      <c r="O27" s="18">
+      <c r="O27" s="3">
         <v>6.7411089999999998</v>
       </c>
-      <c r="P27" s="12">
+      <c r="P27" s="7">
         <v>4.1781940000000004</v>
       </c>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="12"/>
-    </row>
-    <row r="28" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="16"/>
-      <c r="B28" s="26">
+      <c r="Q27" s="38"/>
+      <c r="R27" s="42"/>
+      <c r="S27" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="T27" s="7">
+        <v>1.397E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="50"/>
+      <c r="B28" s="18">
         <v>10</v>
       </c>
       <c r="C28" s="5">
@@ -2171,569 +2387,600 @@
       <c r="E28" s="5">
         <v>69.422079999999994</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="8">
         <v>10.691818</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="11">
         <v>6.7550299999999996</v>
       </c>
-      <c r="H28" s="13">
+      <c r="H28" s="8">
         <v>4.264208</v>
       </c>
       <c r="I28" s="5"/>
-      <c r="J28" s="13"/>
+      <c r="J28" s="8"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="13"/>
+      <c r="L28" s="8"/>
       <c r="M28" s="5">
         <v>69.422079999999994</v>
       </c>
-      <c r="N28" s="13">
+      <c r="N28" s="8">
         <v>10.691818</v>
       </c>
-      <c r="O28" s="19">
+      <c r="O28" s="5">
         <v>6.7550299999999996</v>
       </c>
-      <c r="P28" s="13">
+      <c r="P28" s="8">
         <v>4.264208</v>
       </c>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="13"/>
-    </row>
-    <row r="29" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="7" t="s">
+      <c r="Q28" s="38"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="3">
+        <v>1.2E-5</v>
+      </c>
+      <c r="T28" s="8">
+        <v>1.2539999999999999E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="41">
+      <c r="B29" s="44"/>
+      <c r="C29" s="33">
         <f>AVERAGE(C19:C28)</f>
         <v>8.4109204999999996</v>
       </c>
-      <c r="D29" s="42">
-        <f t="shared" ref="D29" si="7">AVERAGE(D19:D28)</f>
+      <c r="D29" s="34">
+        <f t="shared" ref="D29" si="6">AVERAGE(D19:D28)</f>
         <v>1.2911496999999998</v>
       </c>
-      <c r="E29" s="41">
-        <f t="shared" ref="E29" si="8">AVERAGE(E19:E28)</f>
+      <c r="E29" s="33">
+        <f t="shared" ref="E29" si="7">AVERAGE(E19:E28)</f>
         <v>69.501978600000001</v>
       </c>
-      <c r="F29" s="42">
-        <f t="shared" ref="F29" si="9">AVERAGE(F19:F28)</f>
+      <c r="F29" s="34">
+        <f t="shared" ref="F29" si="8">AVERAGE(F19:F28)</f>
         <v>10.609711700000002</v>
       </c>
-      <c r="G29" s="41">
-        <f t="shared" ref="G29" si="10">AVERAGE(G19:G28)</f>
+      <c r="G29" s="33">
+        <f t="shared" ref="G29" si="9">AVERAGE(G19:G28)</f>
         <v>6.6402970999999997</v>
       </c>
-      <c r="H29" s="42">
-        <f t="shared" ref="H29" si="11">AVERAGE(H19:H28)</f>
+      <c r="H29" s="34">
+        <f t="shared" ref="H29" si="10">AVERAGE(H19:H28)</f>
         <v>4.3155770000000002</v>
       </c>
-      <c r="I29" s="41" t="e">
-        <f t="shared" ref="I29" si="12">AVERAGE(I19:I28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J29" s="42" t="e">
-        <f t="shared" ref="J29" si="13">AVERAGE(J19:J28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K29" s="41" t="e">
-        <f t="shared" ref="K29" si="14">AVERAGE(K19:K28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L29" s="42" t="e">
-        <f t="shared" ref="L29" si="15">AVERAGE(L19:L28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M29" s="41">
-        <f t="shared" ref="M29" si="16">AVERAGE(M19:M28)</f>
+      <c r="I29" s="33" t="e">
+        <f t="shared" ref="I29" si="11">AVERAGE(I19:I28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J29" s="34" t="e">
+        <f t="shared" ref="J29" si="12">AVERAGE(J19:J28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K29" s="33" t="e">
+        <f t="shared" ref="K29" si="13">AVERAGE(K19:K28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L29" s="34" t="e">
+        <f t="shared" ref="L29" si="14">AVERAGE(L19:L28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M29" s="33">
+        <f t="shared" ref="M29" si="15">AVERAGE(M19:M28)</f>
         <v>69.501978600000001</v>
       </c>
-      <c r="N29" s="42">
-        <f t="shared" ref="N29" si="17">AVERAGE(N19:N28)</f>
+      <c r="N29" s="34">
+        <f t="shared" ref="N29" si="16">AVERAGE(N19:N28)</f>
         <v>10.609711700000002</v>
       </c>
-      <c r="O29" s="41">
-        <f t="shared" ref="O29" si="18">AVERAGE(O19:O28)</f>
+      <c r="O29" s="33">
+        <f t="shared" ref="O29" si="17">AVERAGE(O19:O28)</f>
         <v>6.6402970999999997</v>
       </c>
-      <c r="P29" s="42">
-        <f t="shared" ref="P29" si="19">AVERAGE(P19:P28)</f>
+      <c r="P29" s="34">
+        <f t="shared" ref="P29" si="18">AVERAGE(P19:P28)</f>
         <v>4.3155770000000002</v>
       </c>
-      <c r="Q29" s="41" t="e">
-        <f t="shared" ref="Q29" si="20">AVERAGE(Q19:Q28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R29" s="42" t="e">
-        <f t="shared" ref="R29" si="21">AVERAGE(R19:R28)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="7" t="s">
+      <c r="Q29" s="38"/>
+      <c r="R29" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="S29" s="33">
+        <f t="shared" ref="S29" si="19">AVERAGE(S19:S28)</f>
+        <v>1.04E-5</v>
+      </c>
+      <c r="T29" s="34">
+        <f t="shared" ref="T29" si="20">AVERAGE(T19:T28)</f>
+        <v>2.2671999999999996E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="43" t="str">
+      <c r="B30" s="45"/>
+      <c r="C30" s="52" t="str">
         <f>IMDIV(C29,D29)</f>
         <v>6,51428761513866</v>
       </c>
-      <c r="D30" s="44"/>
-      <c r="E30" s="43" t="str">
+      <c r="D30" s="53"/>
+      <c r="E30" s="52" t="str">
         <f>IMDIV(E29,F29)</f>
         <v>6,55078861379428</v>
       </c>
-      <c r="F30" s="44"/>
-      <c r="G30" s="43" t="str">
-        <f t="shared" ref="G30" si="22">IMDIV(G29,H29)</f>
+      <c r="F30" s="53"/>
+      <c r="G30" s="52" t="str">
+        <f>IMDIV(G29,H29)</f>
         <v>1,53868117751114</v>
       </c>
-      <c r="H30" s="44"/>
-      <c r="I30" s="43" t="e">
-        <f t="shared" ref="I30" si="23">IMDIV(I29,J29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J30" s="44"/>
-      <c r="K30" s="43" t="e">
-        <f t="shared" ref="K30" si="24">IMDIV(K29,L29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L30" s="44"/>
-      <c r="M30" s="43" t="str">
-        <f t="shared" ref="M30" si="25">IMDIV(M29,N29)</f>
+      <c r="H30" s="53"/>
+      <c r="I30" s="52" t="e">
+        <f t="shared" ref="I30" si="21">IMDIV(I29,J29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J30" s="53"/>
+      <c r="K30" s="52" t="e">
+        <f t="shared" ref="K30" si="22">IMDIV(K29,L29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L30" s="53"/>
+      <c r="M30" s="52" t="str">
+        <f t="shared" ref="M30" si="23">IMDIV(M29,N29)</f>
         <v>6,55078861379428</v>
       </c>
-      <c r="N30" s="44"/>
-      <c r="O30" s="43" t="str">
-        <f t="shared" ref="O30" si="26">IMDIV(O29,P29)</f>
+      <c r="N30" s="53"/>
+      <c r="O30" s="52" t="str">
+        <f t="shared" ref="O30" si="24">IMDIV(O29,P29)</f>
         <v>1,53868117751114</v>
       </c>
-      <c r="P30" s="44"/>
-      <c r="Q30" s="43" t="e">
-        <f t="shared" ref="Q30" si="27">IMDIV(Q29,R29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R30" s="45"/>
-    </row>
-    <row r="31" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="34" t="s">
+      <c r="P30" s="54"/>
+      <c r="Q30" s="38"/>
+      <c r="R30" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="S30" s="52" t="str">
+        <f t="shared" ref="S30" si="25">IMDIV(S29,T29)</f>
+        <v>0,00458715596330275</v>
+      </c>
+      <c r="T30" s="54"/>
+    </row>
+    <row r="31" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q31" s="39"/>
+    </row>
+    <row r="32" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="36" t="s">
+      <c r="D32" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="35" t="s">
+      <c r="E32" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="36" t="s">
+      <c r="F32" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G32" s="32" t="s">
+      <c r="G32" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H32" s="31" t="s">
+      <c r="H32" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I32" s="32" t="s">
+      <c r="I32" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="J32" s="33" t="s">
+      <c r="J32" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="K32" s="32" t="s">
+      <c r="K32" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="L32" s="33" t="s">
+      <c r="L32" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="M32" s="35" t="s">
+      <c r="M32" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="N32" s="36" t="s">
+      <c r="N32" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="O32" s="32" t="s">
+      <c r="O32" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="P32" s="31" t="s">
+      <c r="P32" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Q32" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="R32" s="33" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="14" t="s">
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="37"/>
+      <c r="T32" s="37"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A33" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="24">
+      <c r="B33" s="16">
         <v>1</v>
       </c>
-      <c r="C33" s="27"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="12"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="7"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="12"/>
+      <c r="J33" s="7"/>
       <c r="K33" s="3"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="28"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="12"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="12"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="15"/>
-      <c r="B34" s="25">
+      <c r="L33" s="7"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="38"/>
+      <c r="R33" s="38"/>
+      <c r="S33" s="38"/>
+      <c r="T33" s="38"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A34" s="49"/>
+      <c r="B34" s="17">
         <v>2</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="4"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="12"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="7"/>
       <c r="I34" s="3"/>
-      <c r="J34" s="12"/>
+      <c r="J34" s="7"/>
       <c r="K34" s="3"/>
-      <c r="L34" s="12"/>
+      <c r="L34" s="7"/>
       <c r="M34" s="3"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="12"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="12"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="15"/>
-      <c r="B35" s="25">
+      <c r="N34" s="7"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="38"/>
+      <c r="R34" s="38"/>
+      <c r="S34" s="38"/>
+      <c r="T34" s="38"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A35" s="49"/>
+      <c r="B35" s="17">
         <v>3</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="4"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="12"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="7"/>
       <c r="I35" s="3"/>
-      <c r="J35" s="12"/>
+      <c r="J35" s="7"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="12"/>
+      <c r="L35" s="7"/>
       <c r="M35" s="3"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="12"/>
-      <c r="Q35" s="3"/>
-      <c r="R35" s="12"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
-      <c r="B36" s="25">
+      <c r="N35" s="7"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="38"/>
+      <c r="R35" s="38"/>
+      <c r="S35" s="38"/>
+      <c r="T35" s="38"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A36" s="49"/>
+      <c r="B36" s="17">
         <v>4</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="4"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="12"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="7"/>
       <c r="I36" s="3"/>
-      <c r="J36" s="12"/>
+      <c r="J36" s="7"/>
       <c r="K36" s="3"/>
-      <c r="L36" s="12"/>
+      <c r="L36" s="7"/>
       <c r="M36" s="3"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="12"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="12"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" s="15"/>
-      <c r="B37" s="25">
+      <c r="N36" s="7"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="38"/>
+      <c r="R36" s="38"/>
+      <c r="S36" s="38"/>
+      <c r="T36" s="38"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A37" s="49"/>
+      <c r="B37" s="17">
         <v>5</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="12"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="7"/>
       <c r="I37" s="3"/>
-      <c r="J37" s="12"/>
+      <c r="J37" s="7"/>
       <c r="K37" s="3"/>
-      <c r="L37" s="12"/>
+      <c r="L37" s="7"/>
       <c r="M37" s="3"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="12"/>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
-      <c r="B38" s="25">
+      <c r="N37" s="7"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="38"/>
+      <c r="R37" s="38"/>
+      <c r="S37" s="38"/>
+      <c r="T37" s="38"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A38" s="49"/>
+      <c r="B38" s="17">
         <v>6</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="4"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="12"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="7"/>
       <c r="I38" s="3"/>
-      <c r="J38" s="12"/>
+      <c r="J38" s="7"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="12"/>
+      <c r="L38" s="7"/>
       <c r="M38" s="3"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="12"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="12"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="25">
+      <c r="N38" s="7"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="38"/>
+      <c r="R38" s="38"/>
+      <c r="S38" s="38"/>
+      <c r="T38" s="38"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A39" s="49"/>
+      <c r="B39" s="17">
         <v>7</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="4"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="12"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="7"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="12"/>
+      <c r="J39" s="7"/>
       <c r="K39" s="3"/>
-      <c r="L39" s="12"/>
+      <c r="L39" s="7"/>
       <c r="M39" s="3"/>
-      <c r="N39" s="12"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="12"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="12"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="25">
+      <c r="N39" s="7"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="38"/>
+      <c r="R39" s="38"/>
+      <c r="S39" s="38"/>
+      <c r="T39" s="38"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A40" s="49"/>
+      <c r="B40" s="17">
         <v>8</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="4"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="12"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="7"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="12"/>
+      <c r="J40" s="7"/>
       <c r="K40" s="3"/>
-      <c r="L40" s="12"/>
+      <c r="L40" s="7"/>
       <c r="M40" s="3"/>
-      <c r="N40" s="12"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="12"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="12"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A41" s="15"/>
-      <c r="B41" s="25">
+      <c r="N40" s="7"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="38"/>
+      <c r="R40" s="38"/>
+      <c r="S40" s="38"/>
+      <c r="T40" s="38"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A41" s="49"/>
+      <c r="B41" s="17">
         <v>9</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="4"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="12"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="7"/>
       <c r="I41" s="3"/>
-      <c r="J41" s="12"/>
+      <c r="J41" s="7"/>
       <c r="K41" s="3"/>
-      <c r="L41" s="12"/>
+      <c r="L41" s="7"/>
       <c r="M41" s="3"/>
-      <c r="N41" s="12"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="12"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="12"/>
-    </row>
-    <row r="42" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="16"/>
-      <c r="B42" s="26">
+      <c r="N41" s="7"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="38"/>
+      <c r="R41" s="38"/>
+      <c r="S41" s="38"/>
+      <c r="T41" s="38"/>
+    </row>
+    <row r="42" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="50"/>
+      <c r="B42" s="18">
         <v>10</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="6"/>
       <c r="E42" s="5"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="13"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="8"/>
       <c r="I42" s="5"/>
-      <c r="J42" s="13"/>
+      <c r="J42" s="8"/>
       <c r="K42" s="5"/>
-      <c r="L42" s="13"/>
+      <c r="L42" s="8"/>
       <c r="M42" s="5"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="19"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="13"/>
-    </row>
-    <row r="43" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="7" t="s">
+      <c r="N42" s="8"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="38"/>
+      <c r="R42" s="38"/>
+      <c r="S42" s="38"/>
+      <c r="T42" s="38"/>
+    </row>
+    <row r="43" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="41" t="e">
+      <c r="B43" s="44"/>
+      <c r="C43" s="33" t="e">
         <f>AVERAGE(C33:C42)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D43" s="42" t="e">
-        <f t="shared" ref="D43" si="28">AVERAGE(D33:D42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E43" s="41" t="e">
-        <f t="shared" ref="E43" si="29">AVERAGE(E33:E42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F43" s="42" t="e">
-        <f t="shared" ref="F43" si="30">AVERAGE(F33:F42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G43" s="41" t="e">
-        <f t="shared" ref="G43" si="31">AVERAGE(G33:G42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H43" s="42" t="e">
-        <f t="shared" ref="H43" si="32">AVERAGE(H33:H42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I43" s="41" t="e">
-        <f t="shared" ref="I43" si="33">AVERAGE(I33:I42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J43" s="42" t="e">
-        <f t="shared" ref="J43" si="34">AVERAGE(J33:J42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K43" s="41" t="e">
-        <f t="shared" ref="K43" si="35">AVERAGE(K33:K42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L43" s="42" t="e">
-        <f t="shared" ref="L43" si="36">AVERAGE(L33:L42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M43" s="41" t="e">
-        <f t="shared" ref="M43" si="37">AVERAGE(M33:M42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N43" s="42" t="e">
-        <f t="shared" ref="N43" si="38">AVERAGE(N33:N42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O43" s="41" t="e">
-        <f t="shared" ref="O43" si="39">AVERAGE(O33:O42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P43" s="42" t="e">
-        <f t="shared" ref="P43" si="40">AVERAGE(P33:P42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q43" s="41" t="e">
-        <f t="shared" ref="Q43" si="41">AVERAGE(Q33:Q42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R43" s="42" t="e">
-        <f t="shared" ref="R43" si="42">AVERAGE(R33:R42)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="7" t="s">
+      <c r="D43" s="34" t="e">
+        <f t="shared" ref="D43" si="26">AVERAGE(D33:D42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E43" s="33" t="e">
+        <f t="shared" ref="E43" si="27">AVERAGE(E33:E42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F43" s="34" t="e">
+        <f t="shared" ref="F43" si="28">AVERAGE(F33:F42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G43" s="33" t="e">
+        <f t="shared" ref="G43" si="29">AVERAGE(G33:G42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H43" s="34" t="e">
+        <f t="shared" ref="H43" si="30">AVERAGE(H33:H42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I43" s="33" t="e">
+        <f t="shared" ref="I43" si="31">AVERAGE(I33:I42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J43" s="34" t="e">
+        <f t="shared" ref="J43" si="32">AVERAGE(J33:J42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K43" s="33" t="e">
+        <f t="shared" ref="K43" si="33">AVERAGE(K33:K42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L43" s="34" t="e">
+        <f t="shared" ref="L43" si="34">AVERAGE(L33:L42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M43" s="33" t="e">
+        <f t="shared" ref="M43" si="35">AVERAGE(M33:M42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N43" s="34" t="e">
+        <f t="shared" ref="N43" si="36">AVERAGE(N33:N42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O43" s="33" t="e">
+        <f t="shared" ref="O43" si="37">AVERAGE(O33:O42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P43" s="34" t="e">
+        <f t="shared" ref="P43" si="38">AVERAGE(P33:P42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="38"/>
+      <c r="S43" s="38"/>
+      <c r="T43" s="38"/>
+    </row>
+    <row r="44" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="43" t="e">
+      <c r="B44" s="45"/>
+      <c r="C44" s="52" t="e">
         <f>IMDIV(C43,D43)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D44" s="44"/>
-      <c r="E44" s="43" t="e">
+      <c r="D44" s="53"/>
+      <c r="E44" s="52" t="e">
         <f>IMDIV(E43,F43)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F44" s="44"/>
-      <c r="G44" s="43" t="e">
-        <f t="shared" ref="G44" si="43">IMDIV(G43,H43)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H44" s="44"/>
-      <c r="I44" s="43" t="e">
-        <f t="shared" ref="I44" si="44">IMDIV(I43,J43)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J44" s="44"/>
-      <c r="K44" s="43" t="e">
-        <f t="shared" ref="K44" si="45">IMDIV(K43,L43)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L44" s="44"/>
-      <c r="M44" s="43" t="e">
-        <f t="shared" ref="M44" si="46">IMDIV(M43,N43)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N44" s="44"/>
-      <c r="O44" s="43" t="e">
-        <f t="shared" ref="O44" si="47">IMDIV(O43,P43)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P44" s="44"/>
-      <c r="Q44" s="43" t="e">
-        <f t="shared" ref="Q44" si="48">IMDIV(Q43,R43)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R44" s="45"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="52" t="e">
+        <f>IMDIV(G43,H43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H44" s="53"/>
+      <c r="I44" s="52" t="e">
+        <f t="shared" ref="I44" si="39">IMDIV(I43,J43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J44" s="53"/>
+      <c r="K44" s="52" t="e">
+        <f t="shared" ref="K44" si="40">IMDIV(K43,L43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L44" s="53"/>
+      <c r="M44" s="52" t="e">
+        <f t="shared" ref="M44" si="41">IMDIV(M43,N43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N44" s="53"/>
+      <c r="O44" s="52" t="e">
+        <f t="shared" ref="O44" si="42">IMDIV(O43,P43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P44" s="54"/>
+      <c r="Q44" s="38"/>
+      <c r="R44" s="38"/>
+      <c r="S44" s="55"/>
+      <c r="T44" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="Q44:R44"/>
+  <mergeCells count="43">
+    <mergeCell ref="S30:T30"/>
+    <mergeCell ref="A33:A42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="S44:T44"/>
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="I44:J44"/>
     <mergeCell ref="K44:L44"/>
     <mergeCell ref="M44:N44"/>
     <mergeCell ref="O44:P44"/>
-    <mergeCell ref="A33:A42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G30:H30"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="K30:L30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="C3:D3"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="A5:A14"/>
     <mergeCell ref="A19:A28"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="A16:B16"/>
@@ -2744,12 +2991,12 @@
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="O16:P16"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="R5:R14"/>
+    <mergeCell ref="R19:R28"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A5:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>